<commit_message>
Made several updates to the shoe to make it easier to assemble.
</commit_message>
<xml_diff>
--- a/BOM-OnlyPoweredBraking.xlsx
+++ b/BOM-OnlyPoweredBraking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Projects\finallyfunctional\vr-shoes-3d-models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D58869-4A3C-4A1C-8FDC-744F8DBA4DFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EF0CFE-CB00-4796-A466-007DD72D8C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{F7647867-DBAA-4F53-AE8E-AF47AE8504CB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F7647867-DBAA-4F53-AE8E-AF47AE8504CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,7 +639,7 @@
       </c>
       <c r="E2">
         <f>D2/D25 * 100</f>
-        <v>3.9371085261408667</v>
+        <v>4.0291986080950259</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -664,7 +664,7 @@
       </c>
       <c r="E3">
         <f>D3/D25 * 100</f>
-        <v>0.7158379138437938</v>
+        <v>0.73258156510818651</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>6</v>
@@ -689,7 +689,7 @@
       </c>
       <c r="E4">
         <f>D4/D25 * 100</f>
-        <v>1.1760194298862328</v>
+        <v>1.2035268569634492</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="E5">
         <f>D5/D25 * 100</f>
-        <v>2.4236226511568448</v>
+        <v>2.4803118704377174</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -739,7 +739,7 @@
       </c>
       <c r="E6">
         <f>D6/D25 * 100</f>
-        <v>0.81810047296433586</v>
+        <v>0.83723607440935621</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>13</v>
@@ -764,7 +764,7 @@
       </c>
       <c r="E7">
         <f>D7/D25 * 100</f>
-        <v>0.81810047296433586</v>
+        <v>0.83723607440935621</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>14</v>
@@ -789,7 +789,7 @@
       </c>
       <c r="E8">
         <f>D8/D25 * 100</f>
-        <v>0.81810047296433586</v>
+        <v>0.83723607440935621</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
@@ -814,7 +814,7 @@
       </c>
       <c r="E9">
         <f>D9/D25 * 100</f>
-        <v>0.81810047296433586</v>
+        <v>0.83723607440935621</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
@@ -839,7 +839,7 @@
       </c>
       <c r="E10">
         <f>D10/D25 * 100</f>
-        <v>7.414035536239294</v>
+        <v>7.5874519243347889</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>58</v>
@@ -864,7 +864,7 @@
       </c>
       <c r="E11">
         <f>D11/D25 * 100</f>
-        <v>13.713409178064682</v>
+        <v>14.03416969728683</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>60</v>
@@ -889,7 +889,7 @@
       </c>
       <c r="E12">
         <f>D12/D25 * 100</f>
-        <v>5.3611146618944128</v>
+        <v>5.4865126501138111</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>53</v>
@@ -914,7 +914,7 @@
       </c>
       <c r="E13">
         <f>D13/D25 * 100</f>
-        <v>3.6814521283395116</v>
+        <v>3.7675623348421019</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>62</v>
@@ -939,7 +939,7 @@
       </c>
       <c r="E14">
         <f>D14/D25 * 100</f>
-        <v>2.7150709446503893</v>
+        <v>2.7785772219460503</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>27</v>
@@ -964,7 +964,7 @@
       </c>
       <c r="E15">
         <f>D15/D25 * 100</f>
-        <v>7.6671353700626348</v>
+        <v>7.8464718348551825</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>40</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="E16">
         <f>D16/D25 * 100</f>
-        <v>4.2413396395244787</v>
+        <v>4.3405457732660055</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>31</v>
@@ -1006,15 +1006,15 @@
         <v>8.94</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>26.82</v>
+        <v>17.88</v>
       </c>
       <c r="E17">
         <f>D17/D25 * 100</f>
-        <v>6.8567045890323408</v>
+        <v>4.6780565657622768</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>42</v>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E18">
         <f>D18/D25 * 100</f>
-        <v>3.650773360603349</v>
+        <v>3.7361659820517512</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>44</v>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="E19">
         <f>D19/D25*100</f>
-        <v>1.1913588137543141</v>
+        <v>1.2192250333586248</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>38</v>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="E20">
         <f>D20/D25*100</f>
-        <v>1.6106353061485366</v>
+        <v>1.6483085214934201</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>45</v>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E21">
         <f>D21/D25*100</f>
-        <v>30.371980058800972</v>
+        <v>31.082389262447347</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>55</v>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D25">
         <f>SUM(D2:D21)</f>
-        <v>391.15000000000003</v>
+        <v>382.21000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>